<commit_message>
Readability and Final Predictions
Started to integrate final predictions
</commit_message>
<xml_diff>
--- a/impact_df.xlsx
+++ b/impact_df.xlsx
@@ -52,28 +52,28 @@
     <t>rank_sum</t>
   </si>
   <si>
+    <t>Coarse Aggregate</t>
+  </si>
+  <si>
     <t>Superplasticizer</t>
   </si>
   <si>
+    <t>None dropped</t>
+  </si>
+  <si>
     <t>Fly Ash</t>
   </si>
   <si>
-    <t>None dropped</t>
-  </si>
-  <si>
     <t>Fine Aggregate</t>
   </si>
   <si>
-    <t>Coarse Aggregate</t>
-  </si>
-  <si>
     <t>Blast Furnace Slag</t>
   </si>
   <si>
+    <t>Water</t>
+  </si>
+  <si>
     <t>Cement</t>
-  </si>
-  <si>
-    <t>Water</t>
   </si>
   <si>
     <t>Age</t>
@@ -483,7 +483,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -492,22 +492,22 @@
         <v>21</v>
       </c>
       <c r="D2">
-        <v>4.103768353880501</v>
+        <v>4.050491135682797</v>
       </c>
       <c r="E2">
-        <v>0.9265430217729018</v>
+        <v>0.9284379529929546</v>
       </c>
       <c r="F2">
-        <v>2.954562577351485</v>
+        <v>3.003496596534652</v>
       </c>
       <c r="G2">
-        <v>0.9882111665072111</v>
+        <v>0.9879620741801166</v>
       </c>
       <c r="H2">
-        <v>1.001906463417187</v>
+        <v>1.001893348561437</v>
       </c>
       <c r="I2">
-        <v>0.964021186873724</v>
+        <v>0.9925850527515795</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -516,15 +516,15 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -533,34 +533,34 @@
         <v>21</v>
       </c>
       <c r="D3">
-        <v>4.104242457094494</v>
+        <v>4.132459056353194</v>
       </c>
       <c r="E3">
-        <v>0.9265260480072419</v>
+        <v>0.9255123108132824</v>
       </c>
       <c r="F3">
-        <v>3.051024597772274</v>
+        <v>2.935236463490096</v>
       </c>
       <c r="G3">
-        <v>0.9883253333045894</v>
+        <v>1.007955006940382</v>
       </c>
       <c r="H3">
-        <v>1.001888109034148</v>
+        <v>0.9987362378136104</v>
       </c>
       <c r="I3">
-        <v>0.9954950274100941</v>
+        <v>0.9700266826715093</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -571,13 +571,13 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>4.152724127157042</v>
+        <v>4.099844762810547</v>
       </c>
       <c r="E4">
-        <v>0.9247799626052476</v>
+        <v>0.9266834182760539</v>
       </c>
       <c r="F4">
-        <v>3.064831580033001</v>
+        <v>3.025933735561053</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -589,54 +589,54 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>4.169322652109075</v>
+        <v>4.103958847360731</v>
       </c>
       <c r="E5">
-        <v>0.9241774487599614</v>
+        <v>0.9265362019921557</v>
       </c>
       <c r="F5">
-        <v>3.026205600247525</v>
+        <v>3.023033364273923</v>
       </c>
       <c r="G5">
-        <v>1.003997020857583</v>
+        <v>1.001003473250378</v>
       </c>
       <c r="H5">
-        <v>0.999348478698015</v>
+        <v>0.9998411363784062</v>
       </c>
       <c r="I5">
-        <v>0.9873970302195008</v>
+        <v>0.9990414954388972</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M5">
         <v>13</v>
@@ -644,40 +644,40 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>4.135883056593922</v>
+        <v>4.153777034439462</v>
       </c>
       <c r="E6">
-        <v>0.9253888242775729</v>
+        <v>0.9247418142654472</v>
       </c>
       <c r="F6">
-        <v>3.085916460396038</v>
+        <v>2.983447813531355</v>
       </c>
       <c r="G6">
-        <v>0.9959445727557517</v>
+        <v>1.013154710665665</v>
       </c>
       <c r="H6">
-        <v>1.000658385450535</v>
+        <v>0.9979047817492852</v>
       </c>
       <c r="I6">
-        <v>1.006879621216514</v>
+        <v>0.9859594010501949</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M6">
         <v>14</v>
@@ -685,43 +685,43 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>4.206533178776816</v>
+        <v>4.15166216429575</v>
       </c>
       <c r="E7">
-        <v>0.9228180014077644</v>
+        <v>0.9248184292453858</v>
       </c>
       <c r="F7">
-        <v>3.018175665222772</v>
+        <v>3.040838129125411</v>
       </c>
       <c r="G7">
-        <v>1.012957531001851</v>
+        <v>1.012638869148226</v>
       </c>
       <c r="H7">
-        <v>0.9978784561984279</v>
+        <v>0.9979874582906235</v>
       </c>
       <c r="I7">
-        <v>0.984777005329041</v>
+        <v>1.004925551868238</v>
       </c>
       <c r="J7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M7">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -729,37 +729,37 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8">
-        <v>4.205325864618109</v>
+        <v>4.160165934010212</v>
       </c>
       <c r="E8">
-        <v>0.9228622989532992</v>
+        <v>0.9245101278954704</v>
       </c>
       <c r="F8">
-        <v>3.081938660272276</v>
+        <v>3.011985715759072</v>
       </c>
       <c r="G8">
-        <v>1.012666802766183</v>
+        <v>1.014713037856173</v>
       </c>
       <c r="H8">
-        <v>0.9979263568313633</v>
+        <v>0.9976547650063421</v>
       </c>
       <c r="I8">
-        <v>1.005581735828724</v>
+        <v>0.9953905071885538</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M8">
         <v>19</v>
@@ -767,84 +767,84 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>4.238237924642816</v>
+        <v>4.194268993510037</v>
       </c>
       <c r="E9">
-        <v>0.921650171638744</v>
+        <v>0.9232673949662336</v>
       </c>
       <c r="F9">
-        <v>3.080837974422439</v>
+        <v>3.00694590552805</v>
       </c>
       <c r="G9">
-        <v>1.020592217269274</v>
+        <v>1.023031172193642</v>
       </c>
       <c r="H9">
-        <v>0.9966156371320086</v>
+        <v>0.9963137105483387</v>
       </c>
       <c r="I9">
-        <v>1.005222601624741</v>
+        <v>0.9937249683263529</v>
       </c>
       <c r="J9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M9">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>4.230393385868057</v>
+        <v>4.211738151216971</v>
       </c>
       <c r="E10">
-        <v>0.9219399380370276</v>
+        <v>0.9226268802636917</v>
       </c>
       <c r="F10">
-        <v>3.120976382013202</v>
+        <v>3.019617780528051</v>
       </c>
       <c r="G10">
-        <v>1.018703206939052</v>
+        <v>1.02729210369656</v>
       </c>
       <c r="H10">
-        <v>0.9969289726388326</v>
+        <v>0.9956225201267669</v>
       </c>
       <c r="I10">
-        <v>1.018319049681548</v>
+        <v>0.9979127252659975</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L10">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="M10">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -852,119 +852,119 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11">
-        <v>4.246411239423498</v>
+        <v>4.285014397749197</v>
       </c>
       <c r="E11">
-        <v>0.9213476896656643</v>
+        <v>0.9199111691575864</v>
       </c>
       <c r="F11">
-        <v>3.087452480404289</v>
+        <v>3.052759179042904</v>
       </c>
       <c r="G11">
-        <v>1.022560398764219</v>
+        <v>1.045165035666304</v>
       </c>
       <c r="H11">
-        <v>0.9962885517870498</v>
+        <v>0.9926919496077029</v>
       </c>
       <c r="I11">
-        <v>1.00738079720878</v>
+        <v>1.008865178760062</v>
       </c>
       <c r="J11">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+      <c r="L11">
         <v>10</v>
       </c>
-      <c r="K11">
-        <v>10</v>
-      </c>
-      <c r="L11">
-        <v>9</v>
-      </c>
       <c r="M11">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12">
-        <v>4.283324093470131</v>
+        <v>4.263833502307265</v>
       </c>
       <c r="E12">
-        <v>0.9199743417775178</v>
+        <v>0.920700973085667</v>
       </c>
       <c r="F12">
-        <v>3.115531353135311</v>
+        <v>3.176064923679864</v>
       </c>
       <c r="G12">
-        <v>1.031449227618811</v>
+        <v>1.039998767998303</v>
       </c>
       <c r="H12">
-        <v>0.9948034981054394</v>
+        <v>0.9935442405978124</v>
       </c>
       <c r="I12">
-        <v>1.016542433663439</v>
+        <v>1.049614830078549</v>
       </c>
       <c r="J12">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K12">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L12">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="M12">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>4.272002270458836</v>
+        <v>4.308306135239357</v>
       </c>
       <c r="E13">
-        <v>0.920396835563418</v>
+        <v>0.9190381369197338</v>
       </c>
       <c r="F13">
-        <v>3.258145988036301</v>
+        <v>3.075126392326729</v>
       </c>
       <c r="G13">
-        <v>1.028722867122756</v>
+        <v>1.050846162352231</v>
       </c>
       <c r="H13">
-        <v>0.9952603568210089</v>
+        <v>0.991749845518394</v>
       </c>
       <c r="I13">
-        <v>1.063075050930276</v>
+        <v>1.016257017193589</v>
       </c>
       <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
         <v>11</v>
-      </c>
-      <c r="K13">
-        <v>11</v>
-      </c>
-      <c r="L13">
-        <v>13</v>
       </c>
       <c r="M13">
         <v>35</v>
@@ -975,28 +975,28 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14">
-        <v>4.441141078966081</v>
+        <v>4.382404036845277</v>
       </c>
       <c r="E14">
-        <v>0.9139686928695299</v>
+        <v>0.9162292868453769</v>
       </c>
       <c r="F14">
-        <v>3.125022767120459</v>
+        <v>3.116809302805279</v>
       </c>
       <c r="G14">
-        <v>1.069452470951035</v>
+        <v>1.068919505586604</v>
       </c>
       <c r="H14">
-        <v>0.9883093598770666</v>
+        <v>0.9887187671382689</v>
       </c>
       <c r="I14">
-        <v>1.019639313128851</v>
+        <v>1.030032239693899</v>
       </c>
       <c r="J14">
         <v>13</v>
@@ -1016,28 +1016,28 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15">
-        <v>4.489702438525837</v>
+        <v>4.434557267547484</v>
       </c>
       <c r="E15">
-        <v>0.9120769996824585</v>
+        <v>0.9142235796427113</v>
       </c>
       <c r="F15">
-        <v>3.321565542491747</v>
+        <v>3.293626031353134</v>
       </c>
       <c r="G15">
-        <v>1.081146327338506</v>
+        <v>1.08164028740139</v>
       </c>
       <c r="H15">
-        <v>0.9862637995669771</v>
+        <v>0.9865543740315088</v>
       </c>
       <c r="I15">
-        <v>1.083767722876303</v>
+        <v>1.088466013860825</v>
       </c>
       <c r="J15">
         <v>14</v>
@@ -1054,31 +1054,31 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D16">
-        <v>4.601227566939889</v>
+        <v>4.509171889731543</v>
       </c>
       <c r="E16">
-        <v>0.907654697362775</v>
+        <v>0.9113127957298434</v>
       </c>
       <c r="F16">
-        <v>3.432878403465346</v>
+        <v>3.382462252475243</v>
       </c>
       <c r="G16">
-        <v>1.108002223612646</v>
+        <v>1.099839664817063</v>
       </c>
       <c r="H16">
-        <v>0.9814817946593176</v>
+        <v>0.9834132970947024</v>
       </c>
       <c r="I16">
-        <v>1.120087128385822</v>
+        <v>1.117824297579367</v>
       </c>
       <c r="J16">
         <v>15</v>
@@ -1087,48 +1087,48 @@
         <v>15</v>
       </c>
       <c r="L16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M16">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>4.740833611771706</v>
+      </c>
+      <c r="E17">
+        <v>0.9019659805735376</v>
+      </c>
+      <c r="F17">
+        <v>3.33203650990099</v>
+      </c>
+      <c r="G17">
+        <v>1.156344663284701</v>
+      </c>
+      <c r="H17">
+        <v>0.9733269882518248</v>
+      </c>
+      <c r="I17">
+        <v>1.10115977449955</v>
+      </c>
+      <c r="J17">
         <v>17</v>
       </c>
-      <c r="D17">
-        <v>4.660568288739842</v>
-      </c>
-      <c r="E17">
-        <v>0.9052574358575456</v>
-      </c>
-      <c r="F17">
-        <v>3.474027898102307</v>
-      </c>
-      <c r="G17">
-        <v>1.122291812803484</v>
-      </c>
-      <c r="H17">
-        <v>0.9788895439595122</v>
-      </c>
-      <c r="I17">
-        <v>1.133513476151567</v>
-      </c>
-      <c r="J17">
-        <v>16</v>
-      </c>
       <c r="K17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L17">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M17">
         <v>49</v>
@@ -1136,81 +1136,81 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D18">
-        <v>4.76862963760023</v>
+        <v>4.671471408825536</v>
       </c>
       <c r="E18">
-        <v>0.9008130422012007</v>
+        <v>0.9048136282364301</v>
       </c>
       <c r="F18">
-        <v>3.540876134488447</v>
+        <v>3.437783725247521</v>
       </c>
       <c r="G18">
-        <v>1.148313610917573</v>
+        <v>1.139426412238868</v>
       </c>
       <c r="H18">
-        <v>0.9740836508432467</v>
+        <v>0.9763999337764032</v>
       </c>
       <c r="I18">
-        <v>1.155324865991599</v>
+        <v>1.136106744455891</v>
       </c>
       <c r="J18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M18">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
       <c r="D19">
-        <v>4.861665125308479</v>
+        <v>4.775368210074311</v>
       </c>
       <c r="E19">
-        <v>0.8969050327842853</v>
+        <v>0.9005325210457283</v>
       </c>
       <c r="F19">
-        <v>3.470525680693069</v>
+        <v>3.419345761138611</v>
       </c>
       <c r="G19">
-        <v>1.170717094717481</v>
+        <v>1.164768054974032</v>
       </c>
       <c r="H19">
-        <v>0.9698577705528628</v>
+        <v>0.9717801174440186</v>
       </c>
       <c r="I19">
-        <v>1.132370764939619</v>
+        <v>1.130013430550096</v>
       </c>
       <c r="J19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M19">
         <v>54</v>
@@ -1218,113 +1218,113 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20">
+        <v>4.800160345013729</v>
+      </c>
+      <c r="E20">
+        <v>0.8994970354415227</v>
+      </c>
+      <c r="F20">
+        <v>3.495488139438944</v>
+      </c>
+      <c r="G20">
+        <v>1.170815146113751</v>
+      </c>
+      <c r="H20">
+        <v>0.970662707135618</v>
+      </c>
+      <c r="I20">
+        <v>1.155176697480069</v>
+      </c>
+      <c r="J20">
         <v>19</v>
       </c>
-      <c r="D20">
-        <v>4.892820449222159</v>
-      </c>
-      <c r="E20">
-        <v>0.895579458640074</v>
-      </c>
-      <c r="F20">
-        <v>3.497125979785479</v>
-      </c>
-      <c r="G20">
-        <v>1.178219476999496</v>
-      </c>
-      <c r="H20">
-        <v>0.9684243764506842</v>
-      </c>
-      <c r="I20">
-        <v>1.141049969130057</v>
-      </c>
-      <c r="J20">
-        <v>20</v>
-      </c>
       <c r="K20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L20">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M20">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>4.916204919345254</v>
+      </c>
+      <c r="E21">
+        <v>0.8945789501598826</v>
+      </c>
+      <c r="F21">
+        <v>3.414795688943895</v>
+      </c>
+      <c r="G21">
+        <v>1.19911977251916</v>
+      </c>
+      <c r="H21">
+        <v>0.965355516800013</v>
+      </c>
+      <c r="I21">
+        <v>1.128509738601642</v>
+      </c>
+      <c r="J21">
+        <v>22</v>
+      </c>
+      <c r="K21">
+        <v>22</v>
+      </c>
+      <c r="L21">
         <v>17</v>
       </c>
-      <c r="D21">
-        <v>4.842333404927021</v>
-      </c>
-      <c r="E21">
-        <v>0.8977232876747164</v>
-      </c>
-      <c r="F21">
-        <v>3.653442398927393</v>
-      </c>
-      <c r="G21">
-        <v>1.166061904584566</v>
-      </c>
-      <c r="H21">
-        <v>0.9707425809115626</v>
-      </c>
-      <c r="I21">
-        <v>1.192053234745138</v>
-      </c>
-      <c r="J21">
-        <v>18</v>
-      </c>
-      <c r="K21">
-        <v>18</v>
-      </c>
-      <c r="L21">
-        <v>23</v>
-      </c>
       <c r="M21">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22">
-        <v>4.931116987521921</v>
+        <v>4.867383404227323</v>
       </c>
       <c r="E22">
-        <v>0.8939384438706917</v>
+        <v>0.8966623700496579</v>
       </c>
       <c r="F22">
-        <v>3.611813428217817</v>
+        <v>3.422675484735972</v>
       </c>
       <c r="G22">
-        <v>1.187441505029078</v>
+        <v>1.187211635030446</v>
       </c>
       <c r="H22">
-        <v>0.9666498843166209</v>
+        <v>0.9676037710027817</v>
       </c>
       <c r="I22">
-        <v>1.178470442470097</v>
+        <v>1.131113825961346</v>
       </c>
       <c r="J22">
         <v>21</v>
@@ -1333,51 +1333,51 @@
         <v>21</v>
       </c>
       <c r="L22">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M22">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D23">
-        <v>4.988434764486028</v>
+        <v>4.842731592159053</v>
       </c>
       <c r="E23">
-        <v>0.8914584605011234</v>
+        <v>0.8977064664639466</v>
       </c>
       <c r="F23">
-        <v>3.556193120874585</v>
+        <v>3.625240924092409</v>
       </c>
       <c r="G23">
-        <v>1.201243957397458</v>
+        <v>1.181198770277155</v>
       </c>
       <c r="H23">
-        <v>0.9639681832960001</v>
+        <v>0.9687304733843038</v>
       </c>
       <c r="I23">
-        <v>1.160322526054203</v>
+        <v>1.198056944039535</v>
       </c>
       <c r="J23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L23">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="M23">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1385,40 +1385,40 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24">
-        <v>5.068727133018576</v>
+        <v>4.989848607450221</v>
       </c>
       <c r="E24">
-        <v>0.8879362355164158</v>
+        <v>0.8913969251913825</v>
       </c>
       <c r="F24">
-        <v>3.601480610561054</v>
+        <v>3.503082508250825</v>
       </c>
       <c r="G24">
-        <v>1.22057882436044</v>
+        <v>1.217082327778078</v>
       </c>
       <c r="H24">
-        <v>0.9601594664907775</v>
+        <v>0.9619217389792986</v>
       </c>
       <c r="I24">
-        <v>1.175099027961032</v>
+        <v>1.157686457929424</v>
       </c>
       <c r="J24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M24">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1429,75 +1429,75 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D25">
-        <v>5.063246872721606</v>
+        <v>4.993705507910927</v>
       </c>
       <c r="E25">
-        <v>0.8881784291017755</v>
+        <v>0.8912289709445234</v>
       </c>
       <c r="F25">
-        <v>3.768709777227721</v>
+        <v>3.657758121905941</v>
       </c>
       <c r="G25">
-        <v>1.219259145968819</v>
+        <v>1.218023070826617</v>
       </c>
       <c r="H25">
-        <v>0.9604213596925695</v>
+        <v>0.9617404966655302</v>
       </c>
       <c r="I25">
-        <v>1.229662928880138</v>
+        <v>1.208803113868499</v>
       </c>
       <c r="J25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L25">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M25">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D26">
-        <v>5.169522544838635</v>
+        <v>5.052719665190942</v>
       </c>
       <c r="E26">
-        <v>0.8834349779673241</v>
+        <v>0.8886429314902133</v>
       </c>
       <c r="F26">
-        <v>3.763605301155116</v>
+        <v>3.790036613036304</v>
       </c>
       <c r="G26">
-        <v>1.244850942790099</v>
+        <v>1.232417312729464</v>
       </c>
       <c r="H26">
-        <v>0.9552920842689451</v>
+        <v>0.9589498570540856</v>
       </c>
       <c r="I26">
-        <v>1.227997429181603</v>
+        <v>1.252518047072691</v>
       </c>
       <c r="J26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L26">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M26">
         <v>77</v>
@@ -1505,43 +1505,43 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="1">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>5.106078419246904</v>
+      </c>
+      <c r="E27">
+        <v>0.8862785617566814</v>
+      </c>
+      <c r="F27">
+        <v>3.713308580858082</v>
+      </c>
+      <c r="G27">
+        <v>1.245432135763735</v>
+      </c>
+      <c r="H27">
+        <v>0.9563984250473163</v>
+      </c>
+      <c r="I27">
+        <v>1.227161235297038</v>
+      </c>
+      <c r="J27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27">
-        <v>5.074215905332365</v>
-      </c>
-      <c r="E27">
-        <v>0.887693403142799</v>
-      </c>
-      <c r="F27">
-        <v>3.82460602310231</v>
-      </c>
-      <c r="G27">
-        <v>1.221900552494966</v>
-      </c>
-      <c r="H27">
-        <v>0.9598968825427725</v>
-      </c>
-      <c r="I27">
-        <v>1.247900879127958</v>
-      </c>
-      <c r="J27">
-        <v>25</v>
-      </c>
       <c r="K27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M27">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1549,28 +1549,28 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28">
-        <v>5.290871085700572</v>
+        <v>5.231596243673429</v>
       </c>
       <c r="E28">
-        <v>0.877898291014909</v>
+        <v>0.8806188326328511</v>
       </c>
       <c r="F28">
-        <v>3.680051335602307</v>
+        <v>3.640326423267325</v>
       </c>
       <c r="G28">
-        <v>1.274072373625913</v>
+        <v>1.276047398459799</v>
       </c>
       <c r="H28">
-        <v>0.9493050525681096</v>
+        <v>0.950290914097828</v>
       </c>
       <c r="I28">
-        <v>1.200735257225026</v>
+        <v>1.20304234705667</v>
       </c>
       <c r="J28">
         <v>27</v>
@@ -1590,28 +1590,28 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D29">
-        <v>5.620222228075904</v>
+        <v>5.551454794335478</v>
       </c>
       <c r="E29">
-        <v>0.8622237502060257</v>
+        <v>0.8655747050230298</v>
       </c>
       <c r="F29">
-        <v>4.200538675742576</v>
+        <v>4.144835292904292</v>
       </c>
       <c r="G29">
-        <v>1.353382034535367</v>
+        <v>1.3540646330545</v>
       </c>
       <c r="H29">
-        <v>0.9323555711317626</v>
+        <v>0.9340565374885987</v>
       </c>
       <c r="I29">
-        <v>1.370561013240847</v>
+        <v>1.369770674153834</v>
       </c>
       <c r="J29">
         <v>28</v>
@@ -1631,28 +1631,28 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
         <v>19</v>
       </c>
-      <c r="C30" t="s">
-        <v>18</v>
-      </c>
       <c r="D30">
-        <v>6.493074719388669</v>
+        <v>6.647465098991774</v>
       </c>
       <c r="E30">
-        <v>0.8161057356226251</v>
+        <v>0.8072566005467648</v>
       </c>
       <c r="F30">
-        <v>4.358176670792077</v>
+        <v>4.318844936056104</v>
       </c>
       <c r="G30">
-        <v>1.563569965297414</v>
+        <v>1.621394341388372</v>
       </c>
       <c r="H30">
-        <v>0.8824863952756172</v>
+        <v>0.8711244688596419</v>
       </c>
       <c r="I30">
-        <v>1.421995485554593</v>
+        <v>1.427276772554745</v>
       </c>
       <c r="J30">
         <v>29</v>
@@ -1675,25 +1675,25 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31">
-        <v>12.42180792169641</v>
+        <v>12.5444823594578</v>
       </c>
       <c r="E31">
-        <v>0.3269660039523823</v>
+        <v>0.3136069570479888</v>
       </c>
       <c r="F31">
-        <v>9.671042076261191</v>
+        <v>9.681661459806691</v>
       </c>
       <c r="G31">
-        <v>2.991243227659426</v>
+        <v>3.059745694092633</v>
       </c>
       <c r="H31">
-        <v>0.3535608654747111</v>
+        <v>0.3384186561052364</v>
       </c>
       <c r="I31">
-        <v>3.155488914714542</v>
+        <v>3.199561624905037</v>
       </c>
       <c r="J31">
         <v>30</v>
@@ -1716,25 +1716,25 @@
         <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D32">
-        <v>12.4935709411705</v>
+        <v>12.56942961582995</v>
       </c>
       <c r="E32">
-        <v>0.3191670639046972</v>
+        <v>0.3108741778661289</v>
       </c>
       <c r="F32">
-        <v>9.763476457891315</v>
+        <v>9.791248988537237</v>
       </c>
       <c r="G32">
-        <v>3.008524178013145</v>
+        <v>3.065830621160712</v>
       </c>
       <c r="H32">
-        <v>0.3451275728396562</v>
+        <v>0.3354696671323423</v>
       </c>
       <c r="I32">
-        <v>3.185648608393087</v>
+        <v>3.235777728199918</v>
       </c>
       <c r="J32">
         <v>31</v>
@@ -1743,39 +1743,39 @@
         <v>31</v>
       </c>
       <c r="L32">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M32">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>12.54851942752958</v>
+        <v>12.68080350563801</v>
       </c>
       <c r="E33">
-        <v>0.3131650956393828</v>
+        <v>0.2986078049772706</v>
       </c>
       <c r="F33">
-        <v>9.732470166637189</v>
+        <v>9.85514585027698</v>
       </c>
       <c r="G33">
-        <v>3.021756091493683</v>
+        <v>3.092996013084409</v>
       </c>
       <c r="H33">
-        <v>0.3386374146312042</v>
+        <v>0.3222328133730747</v>
       </c>
       <c r="I33">
-        <v>3.175531807373374</v>
+        <v>3.256894139636435</v>
       </c>
       <c r="J33">
         <v>32</v>
@@ -1784,51 +1784,51 @@
         <v>32</v>
       </c>
       <c r="L33">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M33">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B34" t="s">
         <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D34">
-        <v>12.55193587378758</v>
+        <v>12.73274963807372</v>
       </c>
       <c r="E34">
-        <v>0.3127910508789803</v>
+        <v>0.2928496149839912</v>
       </c>
       <c r="F34">
-        <v>9.785814640057744</v>
+        <v>9.81522369533827</v>
       </c>
       <c r="G34">
-        <v>3.02257879152224</v>
+        <v>3.105666281214292</v>
       </c>
       <c r="H34">
-        <v>0.3382329457028888</v>
+        <v>0.3160190516074961</v>
       </c>
       <c r="I34">
-        <v>3.192937159683134</v>
+        <v>3.243700805470012</v>
       </c>
       <c r="J34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M34">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -1842,34 +1842,34 @@
         <v>17</v>
       </c>
       <c r="D35">
-        <v>12.58803316254021</v>
+        <v>12.68953724066267</v>
       </c>
       <c r="E35">
-        <v>0.3088327691223374</v>
+        <v>0.2976413231451733</v>
       </c>
       <c r="F35">
-        <v>9.816619320190938</v>
+        <v>9.886930452911351</v>
       </c>
       <c r="G35">
-        <v>3.031271227534681</v>
+        <v>3.09512627301617</v>
       </c>
       <c r="H35">
-        <v>0.3339527040057268</v>
+        <v>0.3211898662208582</v>
       </c>
       <c r="I35">
-        <v>3.202988178582145</v>
+        <v>3.267398203972291</v>
       </c>
       <c r="J35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L35">
         <v>35</v>
       </c>
       <c r="M35">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -1880,25 +1880,25 @@
         <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D36">
-        <v>12.59139923301127</v>
+        <v>12.74426719366783</v>
       </c>
       <c r="E36">
-        <v>0.3084630801273072</v>
+        <v>0.2915697142916468</v>
       </c>
       <c r="F36">
-        <v>9.797835433610315</v>
+        <v>9.867068301361376</v>
       </c>
       <c r="G36">
-        <v>3.032081796782237</v>
+        <v>3.108475547481781</v>
       </c>
       <c r="H36">
-        <v>0.333552945133369</v>
+        <v>0.3146378887776643</v>
       </c>
       <c r="I36">
-        <v>3.196859330686228</v>
+        <v>3.260834229580997</v>
       </c>
       <c r="J36">
         <v>35</v>
@@ -1921,25 +1921,25 @@
         <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D37">
-        <v>12.60714392660955</v>
+        <v>12.750668372726</v>
       </c>
       <c r="E37">
-        <v>0.3067325585084216</v>
+        <v>0.2908578761129557</v>
       </c>
       <c r="F37">
-        <v>9.984531491631298</v>
+        <v>10.02669823049268</v>
       </c>
       <c r="G37">
-        <v>3.035873210109048</v>
+        <v>3.110036869782624</v>
       </c>
       <c r="H37">
-        <v>0.331681665814113</v>
+        <v>0.3138697319674179</v>
       </c>
       <c r="I37">
-        <v>3.257774931803525</v>
+        <v>3.313588170374651</v>
       </c>
       <c r="J37">
         <v>36</v>
@@ -1962,25 +1962,25 @@
         <v>20</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38">
-        <v>12.94020288814548</v>
+        <v>13.04578847474383</v>
       </c>
       <c r="E38">
-        <v>0.2696188536196954</v>
+        <v>0.257651136655893</v>
       </c>
       <c r="F38">
-        <v>10.06593860796793</v>
+        <v>10.07391021481612</v>
       </c>
       <c r="G38">
-        <v>3.116075735328065</v>
+        <v>3.182020107951749</v>
       </c>
       <c r="H38">
-        <v>0.2915491949675657</v>
+        <v>0.2780357688229835</v>
       </c>
       <c r="I38">
-        <v>3.284336625068169</v>
+        <v>3.32919062186544</v>
       </c>
       <c r="J38">
         <v>37</v>

</xml_diff>